<commit_message>
Fix iDA3, LIDA3, CRIDA3_Results duration to 12h and start hour to 12:00
</commit_message>
<xml_diff>
--- a/exso/Files/ReportsInfo.xlsx
+++ b/exso/Files/ReportsInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thanos\Desktop\Admie-Desktop\exso\exso\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED41E64D-9365-4630-8C75-4611E88D0461}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE93557-23D4-40AB-9F0C-60702EC002A3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -2721,27 +2721,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="254">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="252">
     <dxf>
       <fill>
         <patternFill>
@@ -3219,6 +3199,26 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF93CDDD"/>
@@ -3368,26 +3368,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4953,7 +4933,7 @@
   <sheetPr codeName="Sheet1" filterMode="1"/>
   <dimension ref="A1:L300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J106" sqref="J106"/>
     </sheetView>
   </sheetViews>
@@ -11633,789 +11613,789 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="A1:B98 A108:B111">
-    <cfRule type="expression" dxfId="253" priority="254">
+    <cfRule type="expression" dxfId="251" priority="254">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A78:B81">
-    <cfRule type="expression" dxfId="252" priority="255">
+    <cfRule type="expression" dxfId="250" priority="255">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A88:B98 A108:B111">
-    <cfRule type="expression" dxfId="251" priority="256">
+    <cfRule type="expression" dxfId="249" priority="256">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:E98 A108:E111">
-    <cfRule type="expression" dxfId="250" priority="244">
+    <cfRule type="expression" dxfId="248" priority="244">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C98 C108:C111">
-    <cfRule type="expression" dxfId="249" priority="294">
+    <cfRule type="expression" dxfId="247" priority="294">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C78:C81">
-    <cfRule type="expression" dxfId="248" priority="295">
+    <cfRule type="expression" dxfId="246" priority="295">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C88:C98 C108:C111">
-    <cfRule type="expression" dxfId="247" priority="296">
+    <cfRule type="expression" dxfId="245" priority="296">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78:D82">
-    <cfRule type="expression" dxfId="246" priority="310">
+    <cfRule type="expression" dxfId="244" priority="310">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D88:D98 D108:D111">
-    <cfRule type="expression" dxfId="245" priority="311">
+    <cfRule type="expression" dxfId="243" priority="311">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:E98 D108:E111">
-    <cfRule type="expression" dxfId="244" priority="309">
+    <cfRule type="expression" dxfId="242" priority="309">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F108:H111 F1:I2 I3:I120 F3:H98">
-    <cfRule type="expression" dxfId="243" priority="227">
+    <cfRule type="expression" dxfId="241" priority="227">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F108:H111 F2:I2 I3:I120 F3:H98">
-    <cfRule type="expression" dxfId="242" priority="226">
+    <cfRule type="expression" dxfId="240" priority="226">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H78:H81">
-    <cfRule type="expression" dxfId="241" priority="325">
+    <cfRule type="expression" dxfId="239" priority="325">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H88:H98 H108:H111">
-    <cfRule type="expression" dxfId="240" priority="326">
+    <cfRule type="expression" dxfId="238" priority="326">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J108:J111 J2:J98">
-    <cfRule type="cellIs" dxfId="239" priority="368" operator="equal">
+    <cfRule type="cellIs" dxfId="237" priority="368" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="238" priority="369" operator="equal">
+    <cfRule type="cellIs" dxfId="236" priority="369" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:L98 K108:L111">
-    <cfRule type="expression" dxfId="237" priority="354">
+    <cfRule type="expression" dxfId="235" priority="354">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:L98 K108:L111">
-    <cfRule type="expression" dxfId="236" priority="250">
+    <cfRule type="expression" dxfId="234" priority="250">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K78:L81">
-    <cfRule type="expression" dxfId="235" priority="355">
+    <cfRule type="expression" dxfId="233" priority="355">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K88:L98 K108:L111">
-    <cfRule type="expression" dxfId="234" priority="356">
+    <cfRule type="expression" dxfId="232" priority="356">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A99:E99">
-    <cfRule type="expression" dxfId="233" priority="163">
+    <cfRule type="expression" dxfId="231" priority="163">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A99:B99">
-    <cfRule type="expression" dxfId="232" priority="165">
+    <cfRule type="expression" dxfId="230" priority="165">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G99:H99">
-    <cfRule type="expression" dxfId="231" priority="162">
+    <cfRule type="expression" dxfId="229" priority="162">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G99:H99">
-    <cfRule type="expression" dxfId="230" priority="161">
+    <cfRule type="expression" dxfId="228" priority="161">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C99">
-    <cfRule type="expression" dxfId="229" priority="167">
+    <cfRule type="expression" dxfId="227" priority="167">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A103">
-    <cfRule type="expression" dxfId="228" priority="84">
+    <cfRule type="expression" dxfId="226" priority="84">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K99:L99">
-    <cfRule type="expression" dxfId="227" priority="164">
+    <cfRule type="expression" dxfId="225" priority="164">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A101:B101">
-    <cfRule type="expression" dxfId="226" priority="150">
+    <cfRule type="expression" dxfId="224" priority="150">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A99:B99">
-    <cfRule type="expression" dxfId="225" priority="166">
+    <cfRule type="expression" dxfId="223" priority="166">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A101:E101">
-    <cfRule type="expression" dxfId="224" priority="148">
+    <cfRule type="expression" dxfId="222" priority="148">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C101">
-    <cfRule type="expression" dxfId="223" priority="152">
+    <cfRule type="expression" dxfId="221" priority="152">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C99">
-    <cfRule type="expression" dxfId="222" priority="168">
+    <cfRule type="expression" dxfId="220" priority="168">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D99">
-    <cfRule type="expression" dxfId="221" priority="170">
+    <cfRule type="expression" dxfId="219" priority="170">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D99:E99">
-    <cfRule type="expression" dxfId="220" priority="169">
+    <cfRule type="expression" dxfId="218" priority="169">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G101:H101">
-    <cfRule type="expression" dxfId="219" priority="147">
+    <cfRule type="expression" dxfId="217" priority="147">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G101:H101">
-    <cfRule type="expression" dxfId="218" priority="146">
+    <cfRule type="expression" dxfId="216" priority="146">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H99">
-    <cfRule type="expression" dxfId="217" priority="171">
+    <cfRule type="expression" dxfId="215" priority="171">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J99">
-    <cfRule type="cellIs" dxfId="216" priority="174" operator="equal">
+    <cfRule type="cellIs" dxfId="214" priority="174" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="215" priority="175" operator="equal">
+    <cfRule type="cellIs" dxfId="213" priority="175" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K99:L99">
-    <cfRule type="expression" dxfId="214" priority="172">
+    <cfRule type="expression" dxfId="212" priority="172">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K101:L101">
-    <cfRule type="expression" dxfId="213" priority="149">
+    <cfRule type="expression" dxfId="211" priority="149">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K99:L99">
-    <cfRule type="expression" dxfId="212" priority="173">
+    <cfRule type="expression" dxfId="210" priority="173">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A100:E100">
-    <cfRule type="expression" dxfId="211" priority="133">
+    <cfRule type="expression" dxfId="209" priority="133">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A100:B100">
-    <cfRule type="expression" dxfId="210" priority="135">
+    <cfRule type="expression" dxfId="208" priority="135">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G100:H100">
-    <cfRule type="expression" dxfId="209" priority="132">
+    <cfRule type="expression" dxfId="207" priority="132">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G100:H100">
-    <cfRule type="expression" dxfId="208" priority="131">
+    <cfRule type="expression" dxfId="206" priority="131">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C100">
-    <cfRule type="expression" dxfId="207" priority="137">
+    <cfRule type="expression" dxfId="205" priority="137">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K100:L100">
-    <cfRule type="expression" dxfId="206" priority="134">
+    <cfRule type="expression" dxfId="204" priority="134">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A101:B101">
-    <cfRule type="expression" dxfId="205" priority="151">
+    <cfRule type="expression" dxfId="203" priority="151">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C101">
-    <cfRule type="expression" dxfId="204" priority="153">
+    <cfRule type="expression" dxfId="202" priority="153">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D101">
-    <cfRule type="expression" dxfId="203" priority="155">
+    <cfRule type="expression" dxfId="201" priority="155">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D101:E101">
-    <cfRule type="expression" dxfId="202" priority="154">
+    <cfRule type="expression" dxfId="200" priority="154">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H101">
-    <cfRule type="expression" dxfId="201" priority="156">
+    <cfRule type="expression" dxfId="199" priority="156">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J101">
-    <cfRule type="cellIs" dxfId="200" priority="159" operator="equal">
+    <cfRule type="cellIs" dxfId="198" priority="159" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="199" priority="160" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="160" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K101:L101">
-    <cfRule type="expression" dxfId="198" priority="157">
+    <cfRule type="expression" dxfId="196" priority="157">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K101:L101">
-    <cfRule type="expression" dxfId="197" priority="158">
+    <cfRule type="expression" dxfId="195" priority="158">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D102:D104">
-    <cfRule type="expression" dxfId="196" priority="79">
+    <cfRule type="expression" dxfId="194" priority="79">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A104">
-    <cfRule type="expression" dxfId="195" priority="81">
+    <cfRule type="expression" dxfId="193" priority="81">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D102:D104">
-    <cfRule type="expression" dxfId="194" priority="78">
+    <cfRule type="expression" dxfId="192" priority="78">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D102:D104">
-    <cfRule type="expression" dxfId="193" priority="77">
+    <cfRule type="expression" dxfId="191" priority="77">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A106">
-    <cfRule type="expression" dxfId="192" priority="24">
+    <cfRule type="expression" dxfId="190" priority="24">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A104">
-    <cfRule type="expression" dxfId="191" priority="80">
+    <cfRule type="expression" dxfId="189" priority="80">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A100:B100">
-    <cfRule type="expression" dxfId="190" priority="136">
+    <cfRule type="expression" dxfId="188" priority="136">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C100">
-    <cfRule type="expression" dxfId="189" priority="138">
+    <cfRule type="expression" dxfId="187" priority="138">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D100">
-    <cfRule type="expression" dxfId="188" priority="140">
+    <cfRule type="expression" dxfId="186" priority="140">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D100:E100">
-    <cfRule type="expression" dxfId="187" priority="139">
+    <cfRule type="expression" dxfId="185" priority="139">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H100">
-    <cfRule type="expression" dxfId="186" priority="141">
+    <cfRule type="expression" dxfId="184" priority="141">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J100">
-    <cfRule type="cellIs" dxfId="185" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="183" priority="144" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="184" priority="145" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="145" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K100:L100">
-    <cfRule type="expression" dxfId="183" priority="142">
+    <cfRule type="expression" dxfId="181" priority="142">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K100:L100">
-    <cfRule type="expression" dxfId="182" priority="143">
+    <cfRule type="expression" dxfId="180" priority="143">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A102:C102 E102">
-    <cfRule type="expression" dxfId="181" priority="118">
+    <cfRule type="expression" dxfId="179" priority="118">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A102:B102">
-    <cfRule type="expression" dxfId="180" priority="120">
+    <cfRule type="expression" dxfId="178" priority="120">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G102:H102">
-    <cfRule type="expression" dxfId="179" priority="117">
+    <cfRule type="expression" dxfId="177" priority="117">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G102:H102">
-    <cfRule type="expression" dxfId="178" priority="116">
+    <cfRule type="expression" dxfId="176" priority="116">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C102">
-    <cfRule type="expression" dxfId="177" priority="122">
+    <cfRule type="expression" dxfId="175" priority="122">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K102:L102">
-    <cfRule type="expression" dxfId="176" priority="119">
+    <cfRule type="expression" dxfId="174" priority="119">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B104">
-    <cfRule type="expression" dxfId="175" priority="105">
+    <cfRule type="expression" dxfId="173" priority="105">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A102:B102">
-    <cfRule type="expression" dxfId="174" priority="121">
+    <cfRule type="expression" dxfId="172" priority="121">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B104:C104 E104">
-    <cfRule type="expression" dxfId="173" priority="103">
+    <cfRule type="expression" dxfId="171" priority="103">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C104">
-    <cfRule type="expression" dxfId="172" priority="107">
+    <cfRule type="expression" dxfId="170" priority="107">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C102">
-    <cfRule type="expression" dxfId="171" priority="123">
+    <cfRule type="expression" dxfId="169" priority="123">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G105:H105">
-    <cfRule type="expression" dxfId="170" priority="63">
+    <cfRule type="expression" dxfId="168" priority="63">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E102">
-    <cfRule type="expression" dxfId="169" priority="124">
+    <cfRule type="expression" dxfId="167" priority="124">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G104:H104">
-    <cfRule type="expression" dxfId="168" priority="102">
+    <cfRule type="expression" dxfId="166" priority="102">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G104:H104">
-    <cfRule type="expression" dxfId="167" priority="101">
+    <cfRule type="expression" dxfId="165" priority="101">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H102">
-    <cfRule type="expression" dxfId="166" priority="126">
+    <cfRule type="expression" dxfId="164" priority="126">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J102">
-    <cfRule type="cellIs" dxfId="165" priority="129" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="129" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="164" priority="130" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="130" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K102:L102">
-    <cfRule type="expression" dxfId="163" priority="127">
+    <cfRule type="expression" dxfId="161" priority="127">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K104:L104">
-    <cfRule type="expression" dxfId="162" priority="104">
+    <cfRule type="expression" dxfId="160" priority="104">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K102:L102">
-    <cfRule type="expression" dxfId="161" priority="128">
+    <cfRule type="expression" dxfId="159" priority="128">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B103:C103 E103">
-    <cfRule type="expression" dxfId="160" priority="88">
+    <cfRule type="expression" dxfId="158" priority="88">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B103">
-    <cfRule type="expression" dxfId="159" priority="90">
+    <cfRule type="expression" dxfId="157" priority="90">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G103:H103">
-    <cfRule type="expression" dxfId="158" priority="87">
+    <cfRule type="expression" dxfId="156" priority="87">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G103:H103">
-    <cfRule type="expression" dxfId="157" priority="86">
+    <cfRule type="expression" dxfId="155" priority="86">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C103">
-    <cfRule type="expression" dxfId="156" priority="92">
+    <cfRule type="expression" dxfId="154" priority="92">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K103:L103">
-    <cfRule type="expression" dxfId="155" priority="89">
+    <cfRule type="expression" dxfId="153" priority="89">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B104">
-    <cfRule type="expression" dxfId="154" priority="106">
+    <cfRule type="expression" dxfId="152" priority="106">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C104">
-    <cfRule type="expression" dxfId="153" priority="108">
+    <cfRule type="expression" dxfId="151" priority="108">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E104">
-    <cfRule type="expression" dxfId="152" priority="109">
+    <cfRule type="expression" dxfId="150" priority="109">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H104">
-    <cfRule type="expression" dxfId="151" priority="111">
+    <cfRule type="expression" dxfId="149" priority="111">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J104">
-    <cfRule type="cellIs" dxfId="150" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="114" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="149" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="115" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K104:L104">
-    <cfRule type="expression" dxfId="148" priority="112">
+    <cfRule type="expression" dxfId="146" priority="112">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K104:L104">
-    <cfRule type="expression" dxfId="147" priority="113">
+    <cfRule type="expression" dxfId="145" priority="113">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B103">
-    <cfRule type="expression" dxfId="146" priority="91">
+    <cfRule type="expression" dxfId="144" priority="91">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C103">
-    <cfRule type="expression" dxfId="145" priority="93">
+    <cfRule type="expression" dxfId="143" priority="93">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E103">
-    <cfRule type="expression" dxfId="144" priority="94">
+    <cfRule type="expression" dxfId="142" priority="94">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H103">
-    <cfRule type="expression" dxfId="143" priority="96">
+    <cfRule type="expression" dxfId="141" priority="96">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J103">
-    <cfRule type="cellIs" dxfId="142" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="99" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="141" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="100" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K103:L103">
-    <cfRule type="expression" dxfId="140" priority="97">
+    <cfRule type="expression" dxfId="138" priority="97">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K103:L103">
-    <cfRule type="expression" dxfId="139" priority="98">
+    <cfRule type="expression" dxfId="137" priority="98">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A103">
-    <cfRule type="expression" dxfId="138" priority="83">
+    <cfRule type="expression" dxfId="136" priority="83">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A103">
-    <cfRule type="expression" dxfId="137" priority="85">
+    <cfRule type="expression" dxfId="135" priority="85">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A104">
-    <cfRule type="expression" dxfId="136" priority="82">
+    <cfRule type="expression" dxfId="134" priority="82">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F99:F107">
-    <cfRule type="expression" dxfId="135" priority="18">
+    <cfRule type="expression" dxfId="133" priority="18">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A107">
-    <cfRule type="expression" dxfId="134" priority="20">
+    <cfRule type="expression" dxfId="132" priority="20">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F99:F107">
-    <cfRule type="expression" dxfId="133" priority="19">
+    <cfRule type="expression" dxfId="131" priority="19">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D105:D107">
-    <cfRule type="expression" dxfId="132" priority="28">
+    <cfRule type="expression" dxfId="130" priority="28">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D105:D107">
-    <cfRule type="expression" dxfId="131" priority="27">
+    <cfRule type="expression" dxfId="129" priority="27">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D105:D107">
-    <cfRule type="expression" dxfId="130" priority="26">
+    <cfRule type="expression" dxfId="128" priority="26">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A105:C105 E105">
-    <cfRule type="expression" dxfId="129" priority="65">
+    <cfRule type="expression" dxfId="127" priority="65">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A105:B105">
-    <cfRule type="expression" dxfId="128" priority="67">
+    <cfRule type="expression" dxfId="126" priority="67">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G105:H105">
-    <cfRule type="expression" dxfId="127" priority="64">
+    <cfRule type="expression" dxfId="125" priority="64">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C105">
-    <cfRule type="expression" dxfId="126" priority="69">
+    <cfRule type="expression" dxfId="124" priority="69">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K105:L105">
-    <cfRule type="expression" dxfId="125" priority="66">
+    <cfRule type="expression" dxfId="123" priority="66">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B107">
-    <cfRule type="expression" dxfId="124" priority="53">
+    <cfRule type="expression" dxfId="122" priority="53">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A105:B105">
-    <cfRule type="expression" dxfId="123" priority="68">
+    <cfRule type="expression" dxfId="121" priority="68">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B107:C107 E107">
-    <cfRule type="expression" dxfId="122" priority="51">
+    <cfRule type="expression" dxfId="120" priority="51">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C107">
-    <cfRule type="expression" dxfId="121" priority="55">
+    <cfRule type="expression" dxfId="119" priority="55">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C105">
-    <cfRule type="expression" dxfId="120" priority="70">
+    <cfRule type="expression" dxfId="118" priority="70">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E105">
-    <cfRule type="expression" dxfId="119" priority="71">
+    <cfRule type="expression" dxfId="117" priority="71">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G107:H107">
-    <cfRule type="expression" dxfId="118" priority="50">
+    <cfRule type="expression" dxfId="116" priority="50">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G107:H107">
-    <cfRule type="expression" dxfId="117" priority="49">
+    <cfRule type="expression" dxfId="115" priority="49">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H105">
-    <cfRule type="expression" dxfId="116" priority="72">
+    <cfRule type="expression" dxfId="114" priority="72">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J105">
-    <cfRule type="cellIs" dxfId="115" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="75" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="76" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K105:L105">
-    <cfRule type="expression" dxfId="113" priority="73">
+    <cfRule type="expression" dxfId="111" priority="73">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K107:L107">
-    <cfRule type="expression" dxfId="112" priority="52">
+    <cfRule type="expression" dxfId="110" priority="52">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K105:L105">
-    <cfRule type="expression" dxfId="111" priority="74">
+    <cfRule type="expression" dxfId="109" priority="74">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B106:C106 E106">
-    <cfRule type="expression" dxfId="110" priority="37">
+    <cfRule type="expression" dxfId="108" priority="37">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B106">
-    <cfRule type="expression" dxfId="109" priority="39">
+    <cfRule type="expression" dxfId="107" priority="39">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G106:H106">
-    <cfRule type="expression" dxfId="108" priority="36">
+    <cfRule type="expression" dxfId="106" priority="36">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G106:H106">
-    <cfRule type="expression" dxfId="107" priority="35">
+    <cfRule type="expression" dxfId="105" priority="35">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C106">
-    <cfRule type="expression" dxfId="106" priority="41">
+    <cfRule type="expression" dxfId="104" priority="41">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K106:L106">
-    <cfRule type="expression" dxfId="105" priority="38">
+    <cfRule type="expression" dxfId="103" priority="38">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B107">
-    <cfRule type="expression" dxfId="104" priority="54">
+    <cfRule type="expression" dxfId="102" priority="54">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C107">
-    <cfRule type="expression" dxfId="103" priority="56">
+    <cfRule type="expression" dxfId="101" priority="56">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E107">
-    <cfRule type="expression" dxfId="102" priority="57">
+    <cfRule type="expression" dxfId="100" priority="57">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H107">
-    <cfRule type="expression" dxfId="101" priority="58">
+    <cfRule type="expression" dxfId="99" priority="58">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J107">
-    <cfRule type="cellIs" dxfId="100" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="61" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="62" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K107:L107">
-    <cfRule type="expression" dxfId="98" priority="59">
+    <cfRule type="expression" dxfId="96" priority="59">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K107:L107">
-    <cfRule type="expression" dxfId="97" priority="60">
+    <cfRule type="expression" dxfId="95" priority="60">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B106">
-    <cfRule type="expression" dxfId="96" priority="40">
+    <cfRule type="expression" dxfId="94" priority="40">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C106">
-    <cfRule type="expression" dxfId="95" priority="42">
+    <cfRule type="expression" dxfId="93" priority="42">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E106">
-    <cfRule type="expression" dxfId="94" priority="43">
+    <cfRule type="expression" dxfId="92" priority="43">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H106">
-    <cfRule type="expression" dxfId="93" priority="44">
+    <cfRule type="expression" dxfId="91" priority="44">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12523,10 +12503,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J106">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17234,91 +17214,91 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="C1:E60 A62:I109 A2:I60">
-    <cfRule type="expression" dxfId="69" priority="29">
+    <cfRule type="expression" dxfId="67" priority="29">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62:I109 A2:I60">
-    <cfRule type="expression" dxfId="68" priority="30">
+    <cfRule type="expression" dxfId="66" priority="30">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A88:A106 C88:E106">
-    <cfRule type="expression" dxfId="67" priority="32">
+    <cfRule type="expression" dxfId="65" priority="32">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C90">
-    <cfRule type="expression" dxfId="66" priority="114">
+    <cfRule type="expression" dxfId="64" priority="114">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C88:E105">
-    <cfRule type="expression" dxfId="65" priority="93">
+    <cfRule type="expression" dxfId="63" priority="93">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E60 E62:E106">
-    <cfRule type="expression" dxfId="64" priority="28">
+    <cfRule type="expression" dxfId="62" priority="28">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:I1">
-    <cfRule type="expression" dxfId="63" priority="16">
+    <cfRule type="expression" dxfId="61" priority="16">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G25">
-    <cfRule type="expression" dxfId="62" priority="17">
+    <cfRule type="expression" dxfId="60" priority="17">
       <formula>OR(ROW()=CELL("row"),col()=CELL("col"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61:B61">
-    <cfRule type="expression" dxfId="61" priority="9">
+    <cfRule type="expression" dxfId="59" priority="9">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="10">
+    <cfRule type="expression" dxfId="58" priority="10">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61">
-    <cfRule type="expression" dxfId="59" priority="11">
+    <cfRule type="expression" dxfId="57" priority="11">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61:D61 F61:H61">
-    <cfRule type="expression" dxfId="58" priority="4">
+    <cfRule type="expression" dxfId="56" priority="4">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61:D61 F61:H61">
-    <cfRule type="expression" dxfId="57" priority="3">
+    <cfRule type="expression" dxfId="55" priority="3">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E61">
-    <cfRule type="expression" dxfId="56" priority="5">
+    <cfRule type="expression" dxfId="54" priority="5">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="6">
+    <cfRule type="expression" dxfId="53" priority="6">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H61:I61">
-    <cfRule type="expression" dxfId="54" priority="7">
+    <cfRule type="expression" dxfId="52" priority="7">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="8">
+    <cfRule type="expression" dxfId="51" priority="8">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A110:I300">
-    <cfRule type="expression" dxfId="52" priority="1">
+    <cfRule type="expression" dxfId="50" priority="1">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A110:I300">
-    <cfRule type="expression" dxfId="51" priority="2">
+    <cfRule type="expression" dxfId="49" priority="2">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21768,108 +21748,108 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="A2:B94">
-    <cfRule type="expression" dxfId="50" priority="48">
+    <cfRule type="expression" dxfId="48" priority="48">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="49">
+    <cfRule type="expression" dxfId="47" priority="49">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A77:A86 A88:A94">
-    <cfRule type="expression" dxfId="48" priority="50">
+    <cfRule type="expression" dxfId="46" priority="50">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82:C88">
-    <cfRule type="expression" dxfId="47" priority="21">
+    <cfRule type="expression" dxfId="45" priority="21">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:I2 I56:I81 F64:F68 F69:H74 G75:H81 C64:D94 G82:I93 G94:H94 A1:I1 C3:F63 G56:H68 G3:I53 F75:F94">
-    <cfRule type="expression" dxfId="46" priority="20">
+    <cfRule type="expression" dxfId="44" priority="20">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:I2 I56:I81 F64:F68 F69:H74 G75:H81 C64:D94 G82:I93 G94:H94 C3:F63 G56:H68 G3:I53 F75:F94">
-    <cfRule type="expression" dxfId="45" priority="19">
+    <cfRule type="expression" dxfId="43" priority="19">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25:F25">
-    <cfRule type="expression" dxfId="44" priority="22">
+    <cfRule type="expression" dxfId="42" priority="22">
       <formula>OR(ROW()=CELL("row"),col()=CELL("col"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E64:E94">
-    <cfRule type="expression" dxfId="43" priority="30">
+    <cfRule type="expression" dxfId="41" priority="30">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="31">
+    <cfRule type="expression" dxfId="40" priority="31">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G81">
-    <cfRule type="expression" dxfId="41" priority="106">
+    <cfRule type="expression" dxfId="39" priority="106">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="107">
+    <cfRule type="expression" dxfId="38" priority="107">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H94:I94">
-    <cfRule type="expression" dxfId="39" priority="36">
+    <cfRule type="expression" dxfId="37" priority="36">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="37">
+    <cfRule type="expression" dxfId="36" priority="37">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A95:B300">
-    <cfRule type="expression" dxfId="37" priority="9">
+    <cfRule type="expression" dxfId="35" priority="9">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="10">
+    <cfRule type="expression" dxfId="34" priority="10">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A95:A300">
-    <cfRule type="expression" dxfId="35" priority="11">
+    <cfRule type="expression" dxfId="33" priority="11">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F95:H300 C95:D300">
-    <cfRule type="expression" dxfId="34" priority="4">
+    <cfRule type="expression" dxfId="32" priority="4">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F95:H300 C95:D300">
-    <cfRule type="expression" dxfId="33" priority="3">
+    <cfRule type="expression" dxfId="31" priority="3">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E95:E300">
-    <cfRule type="expression" dxfId="32" priority="5">
+    <cfRule type="expression" dxfId="30" priority="5">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="6">
+    <cfRule type="expression" dxfId="29" priority="6">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H95:I300">
-    <cfRule type="expression" dxfId="30" priority="7">
+    <cfRule type="expression" dxfId="28" priority="7">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="8">
+    <cfRule type="expression" dxfId="27" priority="8">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G54:I55">
-    <cfRule type="expression" dxfId="28" priority="2">
+    <cfRule type="expression" dxfId="26" priority="2">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G54:I55">
-    <cfRule type="expression" dxfId="27" priority="1">
+    <cfRule type="expression" dxfId="25" priority="1">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21884,8 +21864,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:I300"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22934,7 +22914,7 @@
         <v>1</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>272</v>
+        <v>326</v>
       </c>
       <c r="D43" s="12" t="s">
         <v>273</v>
@@ -22944,7 +22924,7 @@
         <v>274</v>
       </c>
       <c r="G43" s="12">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H43" s="12" t="s">
         <v>327</v>
@@ -23246,7 +23226,7 @@
         <v>1</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>272</v>
+        <v>326</v>
       </c>
       <c r="D55" s="12" t="s">
         <v>273</v>
@@ -23256,7 +23236,7 @@
         <v>274</v>
       </c>
       <c r="G55" s="12">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H55" s="12" t="s">
         <v>327</v>
@@ -23558,7 +23538,7 @@
         <v>1</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>272</v>
+        <v>326</v>
       </c>
       <c r="D67" s="12" t="s">
         <v>273</v>
@@ -23568,7 +23548,7 @@
         <v>274</v>
       </c>
       <c r="G67" s="12">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H67" s="12" t="s">
         <v>327</v>
@@ -26812,88 +26792,88 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="A2:B107">
-    <cfRule type="expression" dxfId="26" priority="34">
+    <cfRule type="expression" dxfId="24" priority="34">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="35">
+    <cfRule type="expression" dxfId="23" priority="35">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A77:A86 A88:A107">
-    <cfRule type="expression" dxfId="24" priority="36">
+    <cfRule type="expression" dxfId="22" priority="36">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:I1 C2:I107">
-    <cfRule type="expression" dxfId="23" priority="21">
+    <cfRule type="expression" dxfId="21" priority="21">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:I107">
-    <cfRule type="expression" dxfId="22" priority="20">
+    <cfRule type="expression" dxfId="20" priority="20">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E106:E107">
-    <cfRule type="expression" dxfId="21" priority="22">
+    <cfRule type="expression" dxfId="19" priority="22">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A108:B300">
-    <cfRule type="expression" dxfId="20" priority="10">
+    <cfRule type="expression" dxfId="18" priority="10">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="11">
+    <cfRule type="expression" dxfId="17" priority="11">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A108:A300">
-    <cfRule type="expression" dxfId="18" priority="12">
+    <cfRule type="expression" dxfId="16" priority="12">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C109:I109 C108:G108 I108 C112:I112 C110:G111 I110:I111 C114:I300 C113:G113 I113">
-    <cfRule type="expression" dxfId="17" priority="8">
+    <cfRule type="expression" dxfId="15" priority="8">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C109:I109 C108:G108 I108 C112:I112 C110:G111 I110:I111 C114:I300 C113:G113 I113">
-    <cfRule type="expression" dxfId="16" priority="7">
+    <cfRule type="expression" dxfId="14" priority="7">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E108:E300">
-    <cfRule type="expression" dxfId="15" priority="9">
+    <cfRule type="expression" dxfId="13" priority="9">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H108">
-    <cfRule type="expression" dxfId="14" priority="6">
+    <cfRule type="expression" dxfId="12" priority="6">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H108">
-    <cfRule type="expression" dxfId="13" priority="5">
+    <cfRule type="expression" dxfId="11" priority="5">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H110:H111">
-    <cfRule type="expression" dxfId="12" priority="4">
+    <cfRule type="expression" dxfId="10" priority="4">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H110:H111">
-    <cfRule type="expression" dxfId="11" priority="3">
+    <cfRule type="expression" dxfId="9" priority="3">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H113">
-    <cfRule type="expression" dxfId="10" priority="2">
+    <cfRule type="expression" dxfId="8" priority="2">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H113">
-    <cfRule type="expression" dxfId="9" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27914,35 +27894,35 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A108">
-    <cfRule type="expression" dxfId="8" priority="11">
+    <cfRule type="expression" dxfId="6" priority="11">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="12">
+    <cfRule type="expression" dxfId="5" priority="12">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A77:A86">
-    <cfRule type="expression" dxfId="6" priority="13">
+    <cfRule type="expression" dxfId="4" priority="13">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A88:A108">
-    <cfRule type="expression" dxfId="5" priority="18">
+    <cfRule type="expression" dxfId="3" priority="18">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A112:A116">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:C80 B81:B108 C81:C110 B106:C116 A109:B111 A112:C121">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:C80 B81:B108 C81:C111 A109:B111 A112:C121 A1:C1">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27977,7 +27957,7 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="37">
         <f ca="1">NOW()</f>
-        <v>45667.863867708336</v>
+        <v>45680.752327430557</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added support for Crete-ISP equivalent report
</commit_message>
<xml_diff>
--- a/exso/Files/ReportsInfo.xlsx
+++ b/exso/Files/ReportsInfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thanos\Desktop\Admie-Desktop\exso\exso\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.natsikas\Desktop\Admie-Desktop\Projects\exso\exso\exso\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE93557-23D4-40AB-9F0C-60702EC002A3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D2E72F-8D6B-4644-BFC4-7A898FE28E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -26,8 +26,19 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Read Settings'!$A$1:$I$111</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Time Settings'!$A$1:$I$120</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -714,7 +725,8 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>default: None</t>
+          <t>default: None
+Value should be actual excel row</t>
         </r>
       </text>
     </comment>
@@ -1172,7 +1184,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1993" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2000" uniqueCount="337">
   <si>
     <t>Report Name</t>
   </si>
@@ -2181,6 +2193,12 @@
   </si>
   <si>
     <t>MonthlyNTC.txt</t>
+  </si>
+  <si>
+    <t>['Overview','Schedule','Reserves','UnitAvailabilities']</t>
+  </si>
+  <si>
+    <t>DailyDispatchOfCreteElectricalSystem.txt</t>
   </si>
 </sst>
 </file>
@@ -2721,7 +2739,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="252">
+  <dxfs count="116">
     <dxf>
       <fill>
         <patternFill>
@@ -2733,6 +2751,34 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF93CDDD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF93CDDD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF93CDDD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF93CDDD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2823,188 +2869,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFFF99"/>
         </patternFill>
       </fill>
@@ -3027,6 +2891,13 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF93CDDD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3069,55 +2940,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3180,7 +3002,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF93CDDD"/>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3199,22 +3028,23 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFFF99"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FF93CDDD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF93CDDD"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3236,26 +3066,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3360,6 +3170,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF93CDDD"/>
         </patternFill>
       </fill>
@@ -3368,6 +3185,20 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF93CDDD"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3443,13 +3274,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FF93CDDD"/>
         </patternFill>
       </fill>
@@ -3458,89 +3282,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3576,34 +3317,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3687,172 +3400,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFFF99"/>
         </patternFill>
       </fill>
@@ -3875,186 +3422,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4111,200 +3478,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4382,173 +3555,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4634,9 +3640,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4674,7 +3680,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -4780,7 +3786,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4922,7 +3928,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4930,11 +3936,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1" filterMode="1"/>
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L300"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J106" sqref="J106"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5025,7 +4031,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>16</v>
       </c>
@@ -5062,7 +4068,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>20</v>
       </c>
@@ -5099,7 +4105,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>21</v>
       </c>
@@ -5133,7 +4139,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>24</v>
       </c>
@@ -5167,7 +4173,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>26</v>
       </c>
@@ -5200,7 +4206,7 @@
       <c r="K7" s="14"/>
       <c r="L7" s="15"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>27</v>
       </c>
@@ -5233,7 +4239,7 @@
       <c r="K8" s="14"/>
       <c r="L8" s="15"/>
     </row>
-    <row r="9" spans="1:12" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>28</v>
       </c>
@@ -5266,7 +4272,7 @@
       <c r="K9" s="14"/>
       <c r="L9" s="15"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>29</v>
       </c>
@@ -5299,7 +4305,7 @@
       </c>
       <c r="L10" s="15"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>31</v>
       </c>
@@ -5324,15 +4330,14 @@
         <v>1</v>
       </c>
       <c r="J11" s="13" t="b">
-        <f>IF(Metadata!H11="",TRUE(),FALSE())</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" s="14"/>
       <c r="L11" s="15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>33</v>
       </c>
@@ -5349,8 +4354,8 @@
       </c>
       <c r="G12" s="48"/>
       <c r="H12" s="8" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="I12" s="7" t="b">
         <f>IF(Metadata!G12="",TRUE(),FALSE())</f>
@@ -5748,7 +4753,7 @@
       <c r="K23" s="14"/>
       <c r="L23" s="15"/>
     </row>
-    <row r="24" spans="1:12" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
         <v>59</v>
       </c>
@@ -5783,7 +4788,7 @@
       </c>
       <c r="L24" s="15"/>
     </row>
-    <row r="25" spans="1:12" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
         <v>61</v>
       </c>
@@ -5853,7 +4858,7 @@
       <c r="K26" s="14"/>
       <c r="L26" s="15"/>
     </row>
-    <row r="27" spans="1:12" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
         <v>63</v>
       </c>
@@ -5886,7 +4891,7 @@
       <c r="K27" s="14"/>
       <c r="L27" s="15"/>
     </row>
-    <row r="28" spans="1:12" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
         <v>64</v>
       </c>
@@ -5919,7 +4924,7 @@
       <c r="K28" s="14"/>
       <c r="L28" s="15"/>
     </row>
-    <row r="29" spans="1:12" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
         <v>65</v>
       </c>
@@ -5954,7 +4959,7 @@
       </c>
       <c r="L29" s="15"/>
     </row>
-    <row r="30" spans="1:12" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
         <v>67</v>
       </c>
@@ -5987,7 +4992,7 @@
       </c>
       <c r="L30" s="15"/>
     </row>
-    <row r="31" spans="1:12" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
         <v>69</v>
       </c>
@@ -6912,7 +5917,7 @@
       <c r="K57" s="14"/>
       <c r="L57" s="15"/>
     </row>
-    <row r="58" spans="1:12" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="8" t="s">
         <v>86</v>
       </c>
@@ -7056,7 +6061,7 @@
       <c r="K61" s="14"/>
       <c r="L61" s="15"/>
     </row>
-    <row r="62" spans="1:12" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="8" t="s">
         <v>91</v>
       </c>
@@ -7200,7 +6205,7 @@
       <c r="K65" s="14"/>
       <c r="L65" s="15"/>
     </row>
-    <row r="66" spans="1:12" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="8" t="s">
         <v>95</v>
       </c>
@@ -7375,7 +6380,7 @@
       <c r="K70" s="14"/>
       <c r="L70" s="15"/>
     </row>
-    <row r="71" spans="1:12" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="8" t="s">
         <v>100</v>
       </c>
@@ -7406,7 +6411,7 @@
       <c r="K71" s="14"/>
       <c r="L71" s="15"/>
     </row>
-    <row r="72" spans="1:12" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="8" t="s">
         <v>101</v>
       </c>
@@ -7936,7 +6941,7 @@
       <c r="K87" s="14"/>
       <c r="L87" s="15"/>
     </row>
-    <row r="88" spans="1:12" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="8" t="s">
         <v>121</v>
       </c>
@@ -8043,7 +7048,7 @@
       </c>
       <c r="L90" s="15"/>
     </row>
-    <row r="91" spans="1:12" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="8" t="s">
         <v>127</v>
       </c>
@@ -8109,7 +7114,7 @@
       </c>
       <c r="L92" s="15"/>
     </row>
-    <row r="93" spans="1:12" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="8" t="s">
         <v>131</v>
       </c>
@@ -8175,7 +7180,7 @@
       <c r="K94" s="14"/>
       <c r="L94" s="15"/>
     </row>
-    <row r="95" spans="1:12" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="8" t="s">
         <v>133</v>
       </c>
@@ -8210,7 +7215,7 @@
       </c>
       <c r="L95" s="15"/>
     </row>
-    <row r="96" spans="1:12" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="8" t="s">
         <v>135</v>
       </c>
@@ -8245,7 +7250,7 @@
       </c>
       <c r="L96" s="15"/>
     </row>
-    <row r="97" spans="1:12" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="8" t="s">
         <v>136</v>
       </c>
@@ -8280,7 +7285,7 @@
       </c>
       <c r="L97" s="15"/>
     </row>
-    <row r="98" spans="1:12" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="8" t="s">
         <v>138</v>
       </c>
@@ -8315,7 +7320,7 @@
       </c>
       <c r="L98" s="15"/>
     </row>
-    <row r="99" spans="1:12" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="8" t="s">
         <v>139</v>
       </c>
@@ -8350,7 +7355,7 @@
       </c>
       <c r="L99" s="15"/>
     </row>
-    <row r="100" spans="1:12" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="8" t="s">
         <v>140</v>
       </c>
@@ -8453,7 +7458,7 @@
       </c>
       <c r="L102" s="15"/>
     </row>
-    <row r="103" spans="1:12" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="8" t="s">
         <v>146</v>
       </c>
@@ -8593,7 +7598,7 @@
       </c>
       <c r="L106" s="15"/>
     </row>
-    <row r="107" spans="1:12" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="8" t="s">
         <v>154</v>
       </c>
@@ -8628,7 +7633,7 @@
       </c>
       <c r="L107" s="15"/>
     </row>
-    <row r="108" spans="1:12" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="8" t="s">
         <v>156</v>
       </c>
@@ -8663,7 +7668,7 @@
       </c>
       <c r="L108" s="15"/>
     </row>
-    <row r="109" spans="1:12" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="8" t="s">
         <v>158</v>
       </c>
@@ -8698,7 +7703,7 @@
       </c>
       <c r="L109" s="15"/>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="8" t="s">
         <v>160</v>
       </c>
@@ -8733,7 +7738,7 @@
       </c>
       <c r="L110" s="15"/>
     </row>
-    <row r="111" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="8" t="s">
         <v>162</v>
       </c>
@@ -8768,7 +7773,7 @@
       </c>
       <c r="L111" s="15"/>
     </row>
-    <row r="112" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="8" t="s">
         <v>110</v>
       </c>
@@ -8803,7 +7808,7 @@
       </c>
       <c r="L112" s="15"/>
     </row>
-    <row r="113" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="8" t="s">
         <v>165</v>
       </c>
@@ -8838,7 +7843,7 @@
       </c>
       <c r="L113" s="15"/>
     </row>
-    <row r="114" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="8" t="s">
         <v>167</v>
       </c>
@@ -8869,7 +7874,7 @@
       <c r="K114" s="14"/>
       <c r="L114" s="15"/>
     </row>
-    <row r="115" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="8" t="s">
         <v>168</v>
       </c>
@@ -8904,7 +7909,7 @@
       </c>
       <c r="L115" s="15"/>
     </row>
-    <row r="116" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="8" t="s">
         <v>169</v>
       </c>
@@ -8939,7 +7944,7 @@
       </c>
       <c r="L116" s="15"/>
     </row>
-    <row r="117" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="8" t="s">
         <v>170</v>
       </c>
@@ -8974,7 +7979,7 @@
       <c r="K117" s="14"/>
       <c r="L117" s="15"/>
     </row>
-    <row r="118" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="8" t="s">
         <v>171</v>
       </c>
@@ -9009,7 +8014,7 @@
       <c r="K118" s="14"/>
       <c r="L118" s="15"/>
     </row>
-    <row r="119" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="8" t="s">
         <v>172</v>
       </c>
@@ -9046,7 +8051,7 @@
       </c>
       <c r="L119" s="15"/>
     </row>
-    <row r="120" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" s="8" t="s">
         <v>174</v>
       </c>
@@ -11603,911 +10608,321 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:L120" xr:uid="{D0972C50-907B-4A2C-82F0-ED51F06329AA}">
-    <filterColumn colId="9">
-      <filters>
-        <filter val="TRUE"/>
-      </filters>
-    </filterColumn>
-    <sortState ref="A2:L120">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L120">
       <sortCondition ref="A2:A120"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="A1:B98 A108:B111">
-    <cfRule type="expression" dxfId="251" priority="254">
+  <conditionalFormatting sqref="A103">
+    <cfRule type="expression" dxfId="115" priority="85">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="114" priority="84">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A78:B81">
-    <cfRule type="expression" dxfId="250" priority="255">
+  <conditionalFormatting sqref="A104">
+    <cfRule type="expression" dxfId="113" priority="81">
+      <formula>COLUMN()=CELL("col")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="112" priority="80">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A88:B98 A108:B111">
-    <cfRule type="expression" dxfId="249" priority="256">
+  <conditionalFormatting sqref="A106">
+    <cfRule type="expression" dxfId="111" priority="24">
+      <formula>COLUMN()=CELL("col")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="110" priority="25">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:E98 A108:E111">
-    <cfRule type="expression" dxfId="248" priority="244">
+  <conditionalFormatting sqref="A107">
+    <cfRule type="expression" dxfId="109" priority="20">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="108" priority="21">
+      <formula>COLUMN()=CELL("col")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A78:C81">
+    <cfRule type="expression" dxfId="107" priority="255">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C98 C108:C111">
-    <cfRule type="expression" dxfId="247" priority="294">
+  <conditionalFormatting sqref="A102:C102">
+    <cfRule type="expression" dxfId="106" priority="121">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="105" priority="120">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C78:C81">
-    <cfRule type="expression" dxfId="246" priority="295">
+  <conditionalFormatting sqref="A102:C104">
+    <cfRule type="expression" dxfId="104" priority="82">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C88:C98 C108:C111">
-    <cfRule type="expression" dxfId="245" priority="296">
+  <conditionalFormatting sqref="A105:C105">
+    <cfRule type="expression" dxfId="103" priority="67">
+      <formula>COLUMN()=CELL("col")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="102" priority="68">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D78:D82">
-    <cfRule type="expression" dxfId="244" priority="310">
+  <conditionalFormatting sqref="A88:D101">
+    <cfRule type="expression" dxfId="101" priority="136">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D88:D98 D108:D111">
-    <cfRule type="expression" dxfId="243" priority="311">
+  <conditionalFormatting sqref="A108:D111">
+    <cfRule type="expression" dxfId="100" priority="256">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:E98 D108:E111">
-    <cfRule type="expression" dxfId="242" priority="309">
+  <conditionalFormatting sqref="A112:D300">
+    <cfRule type="expression" dxfId="99" priority="8">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:E101">
+    <cfRule type="expression" dxfId="98" priority="135">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F108:H111 F1:I2 I3:I120 F3:H98">
-    <cfRule type="expression" dxfId="241" priority="227">
+  <conditionalFormatting sqref="A2:E101">
+    <cfRule type="expression" dxfId="97" priority="133">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A105:E107">
+    <cfRule type="expression" dxfId="96" priority="22">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A112:E300">
+    <cfRule type="expression" dxfId="95" priority="5">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="94" priority="7">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F108:H111 F2:I2 I3:I120 F3:H98">
-    <cfRule type="expression" dxfId="240" priority="226">
+  <conditionalFormatting sqref="B103:C104">
+    <cfRule type="expression" dxfId="93" priority="90">
+      <formula>COLUMN()=CELL("col")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="92" priority="91">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B106:C107">
+    <cfRule type="expression" dxfId="91" priority="40">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="90" priority="39">
+      <formula>COLUMN()=CELL("col")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D78:D82">
+    <cfRule type="expression" dxfId="89" priority="310">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D102:D104">
+    <cfRule type="expression" dxfId="88" priority="78">
+      <formula>COLUMN()=CELL("col")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D102:D107">
+    <cfRule type="expression" dxfId="87" priority="28">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D102:E104">
+    <cfRule type="expression" dxfId="86" priority="79">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D105:E107">
+    <cfRule type="expression" dxfId="85" priority="27">
+      <formula>COLUMN()=CELL("col")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E102:E104">
+    <cfRule type="expression" dxfId="84" priority="94">
+      <formula>COLUMN()=CELL("col")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:H107">
+    <cfRule type="expression" dxfId="83" priority="19">
+      <formula>COLUMN()=CELL("col")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="82" priority="18">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F112:H120 F121:I300">
+    <cfRule type="expression" dxfId="81" priority="3">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="80" priority="4">
+      <formula>COLUMN()=CELL("col")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:I2 I3:I120 A108:H111">
+    <cfRule type="expression" dxfId="79" priority="227">
+      <formula>COLUMN()=CELL("col")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:I2 I3:I120 A108:H111">
+    <cfRule type="expression" dxfId="78" priority="226">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H78:H81">
-    <cfRule type="expression" dxfId="239" priority="325">
+    <cfRule type="expression" dxfId="77" priority="325">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H88:H98 H108:H111">
-    <cfRule type="expression" dxfId="238" priority="326">
+  <conditionalFormatting sqref="H88:H107">
+    <cfRule type="expression" dxfId="76" priority="44">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J108:J111 J2:J98">
-    <cfRule type="cellIs" dxfId="237" priority="368" operator="equal">
+  <conditionalFormatting sqref="H108:H111">
+    <cfRule type="expression" dxfId="75" priority="326">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H112:H120 H121:I300">
+    <cfRule type="expression" dxfId="74" priority="13">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J300">
+    <cfRule type="cellIs" dxfId="73" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="236" priority="369" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:L98 K108:L111">
-    <cfRule type="expression" dxfId="235" priority="354">
+    <cfRule type="expression" dxfId="71" priority="354">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:L98 K108:L111">
-    <cfRule type="expression" dxfId="234" priority="250">
+  <conditionalFormatting sqref="K2:L99">
+    <cfRule type="expression" dxfId="70" priority="173">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K78:L81">
-    <cfRule type="expression" dxfId="233" priority="355">
+    <cfRule type="expression" dxfId="69" priority="355">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K88:L98 K108:L111">
-    <cfRule type="expression" dxfId="232" priority="356">
+    <cfRule type="expression" dxfId="68" priority="356">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A99:E99">
-    <cfRule type="expression" dxfId="231" priority="163">
+  <conditionalFormatting sqref="K99:L99">
+    <cfRule type="expression" dxfId="67" priority="172">
+      <formula>COLUMN()=CELL("col")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K99:L101">
+    <cfRule type="expression" dxfId="66" priority="143">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A99:B99">
-    <cfRule type="expression" dxfId="230" priority="165">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G99:H99">
-    <cfRule type="expression" dxfId="229" priority="162">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G99:H99">
-    <cfRule type="expression" dxfId="228" priority="161">
+  <conditionalFormatting sqref="K100:L100">
+    <cfRule type="expression" dxfId="65" priority="134">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C99">
-    <cfRule type="expression" dxfId="227" priority="167">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A103">
-    <cfRule type="expression" dxfId="226" priority="84">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K99:L99">
-    <cfRule type="expression" dxfId="225" priority="164">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A101:B101">
-    <cfRule type="expression" dxfId="224" priority="150">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A99:B99">
-    <cfRule type="expression" dxfId="223" priority="166">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A101:E101">
-    <cfRule type="expression" dxfId="222" priority="148">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C101">
-    <cfRule type="expression" dxfId="221" priority="152">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C99">
-    <cfRule type="expression" dxfId="220" priority="168">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D99">
-    <cfRule type="expression" dxfId="219" priority="170">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D99:E99">
-    <cfRule type="expression" dxfId="218" priority="169">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G101:H101">
-    <cfRule type="expression" dxfId="217" priority="147">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G101:H101">
-    <cfRule type="expression" dxfId="216" priority="146">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H99">
-    <cfRule type="expression" dxfId="215" priority="171">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J99">
-    <cfRule type="cellIs" dxfId="214" priority="174" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="213" priority="175" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K99:L99">
-    <cfRule type="expression" dxfId="212" priority="172">
+    <cfRule type="expression" dxfId="64" priority="142">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K101:L101">
-    <cfRule type="expression" dxfId="211" priority="149">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K99:L99">
-    <cfRule type="expression" dxfId="210" priority="173">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A100:E100">
-    <cfRule type="expression" dxfId="209" priority="133">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A100:B100">
-    <cfRule type="expression" dxfId="208" priority="135">
+    <cfRule type="expression" dxfId="63" priority="157">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G100:H100">
-    <cfRule type="expression" dxfId="207" priority="132">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G100:H100">
-    <cfRule type="expression" dxfId="206" priority="131">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C100">
-    <cfRule type="expression" dxfId="205" priority="137">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K100:L100">
-    <cfRule type="expression" dxfId="204" priority="134">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A101:B101">
-    <cfRule type="expression" dxfId="203" priority="151">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C101">
-    <cfRule type="expression" dxfId="202" priority="153">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D101">
-    <cfRule type="expression" dxfId="201" priority="155">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D101:E101">
-    <cfRule type="expression" dxfId="200" priority="154">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H101">
-    <cfRule type="expression" dxfId="199" priority="156">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J101">
-    <cfRule type="cellIs" dxfId="198" priority="159" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="197" priority="160" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K101:L101">
-    <cfRule type="expression" dxfId="196" priority="157">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K101:L101">
-    <cfRule type="expression" dxfId="195" priority="158">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D102:D104">
-    <cfRule type="expression" dxfId="194" priority="79">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A104">
-    <cfRule type="expression" dxfId="193" priority="81">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D102:D104">
-    <cfRule type="expression" dxfId="192" priority="78">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D102:D104">
-    <cfRule type="expression" dxfId="191" priority="77">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A106">
-    <cfRule type="expression" dxfId="190" priority="24">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A104">
-    <cfRule type="expression" dxfId="189" priority="80">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A100:B100">
-    <cfRule type="expression" dxfId="188" priority="136">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C100">
-    <cfRule type="expression" dxfId="187" priority="138">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D100">
-    <cfRule type="expression" dxfId="186" priority="140">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D100:E100">
-    <cfRule type="expression" dxfId="185" priority="139">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H100">
-    <cfRule type="expression" dxfId="184" priority="141">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J100">
-    <cfRule type="cellIs" dxfId="183" priority="144" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="182" priority="145" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K100:L100">
-    <cfRule type="expression" dxfId="181" priority="142">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K100:L100">
-    <cfRule type="expression" dxfId="180" priority="143">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A102:C102 E102">
-    <cfRule type="expression" dxfId="179" priority="118">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A102:B102">
-    <cfRule type="expression" dxfId="178" priority="120">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G102:H102">
-    <cfRule type="expression" dxfId="177" priority="117">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G102:H102">
-    <cfRule type="expression" dxfId="176" priority="116">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C102">
-    <cfRule type="expression" dxfId="175" priority="122">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K102:L102">
-    <cfRule type="expression" dxfId="174" priority="119">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B104">
-    <cfRule type="expression" dxfId="173" priority="105">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A102:B102">
-    <cfRule type="expression" dxfId="172" priority="121">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B104:C104 E104">
-    <cfRule type="expression" dxfId="171" priority="103">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C104">
-    <cfRule type="expression" dxfId="170" priority="107">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C102">
-    <cfRule type="expression" dxfId="169" priority="123">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G105:H105">
-    <cfRule type="expression" dxfId="168" priority="63">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E102">
-    <cfRule type="expression" dxfId="167" priority="124">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G104:H104">
-    <cfRule type="expression" dxfId="166" priority="102">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G104:H104">
-    <cfRule type="expression" dxfId="165" priority="101">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H102">
-    <cfRule type="expression" dxfId="164" priority="126">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J102">
-    <cfRule type="cellIs" dxfId="163" priority="129" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="162" priority="130" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K102:L102">
-    <cfRule type="expression" dxfId="161" priority="127">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K104:L104">
-    <cfRule type="expression" dxfId="160" priority="104">
+    <cfRule type="expression" dxfId="62" priority="158">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K102:L102">
-    <cfRule type="expression" dxfId="159" priority="128">
+    <cfRule type="expression" dxfId="61" priority="127">
+      <formula>COLUMN()=CELL("col")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="60" priority="128">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B103:C103 E103">
-    <cfRule type="expression" dxfId="158" priority="88">
+  <conditionalFormatting sqref="K102:L104">
+    <cfRule type="expression" dxfId="59" priority="98">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B103">
-    <cfRule type="expression" dxfId="157" priority="90">
+  <conditionalFormatting sqref="K103:L103">
+    <cfRule type="expression" dxfId="58" priority="97">
+      <formula>COLUMN()=CELL("col")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="57" priority="89">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K104:L104">
+    <cfRule type="expression" dxfId="56" priority="112">
+      <formula>COLUMN()=CELL("col")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="55" priority="113">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K105:L105">
+    <cfRule type="expression" dxfId="54" priority="74">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="53" priority="73">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G103:H103">
-    <cfRule type="expression" dxfId="156" priority="87">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G103:H103">
-    <cfRule type="expression" dxfId="155" priority="86">
+  <conditionalFormatting sqref="K105:L107">
+    <cfRule type="expression" dxfId="52" priority="46">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C103">
-    <cfRule type="expression" dxfId="154" priority="92">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K103:L103">
-    <cfRule type="expression" dxfId="153" priority="89">
+  <conditionalFormatting sqref="K106:L106">
+    <cfRule type="expression" dxfId="51" priority="38">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B104">
-    <cfRule type="expression" dxfId="152" priority="106">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C104">
-    <cfRule type="expression" dxfId="151" priority="108">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E104">
-    <cfRule type="expression" dxfId="150" priority="109">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H104">
-    <cfRule type="expression" dxfId="149" priority="111">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J104">
-    <cfRule type="cellIs" dxfId="148" priority="114" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="147" priority="115" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K104:L104">
-    <cfRule type="expression" dxfId="146" priority="112">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K104:L104">
-    <cfRule type="expression" dxfId="145" priority="113">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B103">
-    <cfRule type="expression" dxfId="144" priority="91">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C103">
-    <cfRule type="expression" dxfId="143" priority="93">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E103">
-    <cfRule type="expression" dxfId="142" priority="94">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H103">
-    <cfRule type="expression" dxfId="141" priority="96">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J103">
-    <cfRule type="cellIs" dxfId="140" priority="99" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="139" priority="100" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K103:L103">
-    <cfRule type="expression" dxfId="138" priority="97">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K103:L103">
-    <cfRule type="expression" dxfId="137" priority="98">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A103">
-    <cfRule type="expression" dxfId="136" priority="83">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A103">
-    <cfRule type="expression" dxfId="135" priority="85">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A104">
-    <cfRule type="expression" dxfId="134" priority="82">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F99:F107">
-    <cfRule type="expression" dxfId="133" priority="18">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A107">
-    <cfRule type="expression" dxfId="132" priority="20">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F99:F107">
-    <cfRule type="expression" dxfId="131" priority="19">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D105:D107">
-    <cfRule type="expression" dxfId="130" priority="28">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D105:D107">
-    <cfRule type="expression" dxfId="129" priority="27">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D105:D107">
-    <cfRule type="expression" dxfId="128" priority="26">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A105:C105 E105">
-    <cfRule type="expression" dxfId="127" priority="65">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A105:B105">
-    <cfRule type="expression" dxfId="126" priority="67">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G105:H105">
-    <cfRule type="expression" dxfId="125" priority="64">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C105">
-    <cfRule type="expression" dxfId="124" priority="69">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K105:L105">
-    <cfRule type="expression" dxfId="123" priority="66">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B107">
-    <cfRule type="expression" dxfId="122" priority="53">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A105:B105">
-    <cfRule type="expression" dxfId="121" priority="68">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B107:C107 E107">
-    <cfRule type="expression" dxfId="120" priority="51">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C107">
-    <cfRule type="expression" dxfId="119" priority="55">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C105">
-    <cfRule type="expression" dxfId="118" priority="70">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E105">
-    <cfRule type="expression" dxfId="117" priority="71">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G107:H107">
-    <cfRule type="expression" dxfId="116" priority="50">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G107:H107">
-    <cfRule type="expression" dxfId="115" priority="49">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H105">
-    <cfRule type="expression" dxfId="114" priority="72">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J105">
-    <cfRule type="cellIs" dxfId="113" priority="75" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="76" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K105:L105">
-    <cfRule type="expression" dxfId="111" priority="73">
+    <cfRule type="expression" dxfId="50" priority="45">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K107:L107">
-    <cfRule type="expression" dxfId="110" priority="52">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K105:L105">
-    <cfRule type="expression" dxfId="109" priority="74">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B106:C106 E106">
-    <cfRule type="expression" dxfId="108" priority="37">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B106">
-    <cfRule type="expression" dxfId="107" priority="39">
+    <cfRule type="expression" dxfId="49" priority="59">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G106:H106">
-    <cfRule type="expression" dxfId="106" priority="36">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G106:H106">
-    <cfRule type="expression" dxfId="105" priority="35">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C106">
-    <cfRule type="expression" dxfId="104" priority="41">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K106:L106">
-    <cfRule type="expression" dxfId="103" priority="38">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B107">
-    <cfRule type="expression" dxfId="102" priority="54">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C107">
-    <cfRule type="expression" dxfId="101" priority="56">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E107">
-    <cfRule type="expression" dxfId="100" priority="57">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H107">
-    <cfRule type="expression" dxfId="99" priority="58">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J107">
-    <cfRule type="cellIs" dxfId="98" priority="61" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="62" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K107:L107">
-    <cfRule type="expression" dxfId="96" priority="59">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K107:L107">
-    <cfRule type="expression" dxfId="95" priority="60">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B106">
-    <cfRule type="expression" dxfId="94" priority="40">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C106">
-    <cfRule type="expression" dxfId="93" priority="42">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E106">
-    <cfRule type="expression" dxfId="92" priority="43">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H106">
-    <cfRule type="expression" dxfId="91" priority="44">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K106:L106">
-    <cfRule type="expression" dxfId="90" priority="45">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K106:L106">
-    <cfRule type="expression" dxfId="89" priority="46">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A106">
-    <cfRule type="expression" dxfId="88" priority="23">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A106">
-    <cfRule type="expression" dxfId="87" priority="25">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A107">
-    <cfRule type="expression" dxfId="86" priority="21">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A107">
-    <cfRule type="expression" dxfId="85" priority="22">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A112:B300">
-    <cfRule type="expression" dxfId="84" priority="7">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A112:B300">
-    <cfRule type="expression" dxfId="83" priority="8">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A112:E300">
-    <cfRule type="expression" dxfId="82" priority="5">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C112:C300">
-    <cfRule type="expression" dxfId="81" priority="9">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C112:C300">
-    <cfRule type="expression" dxfId="80" priority="10">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D112:D300">
-    <cfRule type="expression" dxfId="79" priority="12">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D112:E300">
-    <cfRule type="expression" dxfId="78" priority="11">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F121:I300 F112:H120">
-    <cfRule type="expression" dxfId="77" priority="4">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F121:I300 F112:H120">
-    <cfRule type="expression" dxfId="76" priority="3">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H121:I300 H112:H120">
-    <cfRule type="expression" dxfId="75" priority="13">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J112:J300">
-    <cfRule type="cellIs" dxfId="74" priority="16" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="17" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K112:L300">
-    <cfRule type="expression" dxfId="72" priority="14">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K112:L300">
-    <cfRule type="expression" dxfId="71" priority="6">
+  <conditionalFormatting sqref="K107:L111">
+    <cfRule type="expression" dxfId="48" priority="60">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K112:L300">
-    <cfRule type="expression" dxfId="70" priority="15">
+    <cfRule type="expression" dxfId="47" priority="15">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J106">
-    <cfRule type="cellIs" dxfId="69" priority="1" operator="equal">
-      <formula>1</formula>
+    <cfRule type="expression" dxfId="46" priority="14">
+      <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="2" operator="equal">
-      <formula>0</formula>
+    <cfRule type="expression" dxfId="45" priority="6">
+      <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -12522,7 +10937,7 @@
   <dimension ref="A1:I300"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12745,13 +11160,23 @@
         <f>Metadata!A11=A11</f>
         <v>1</v>
       </c>
-      <c r="C11" s="8"/>
+      <c r="C11" s="8" t="s">
+        <v>185</v>
+      </c>
       <c r="D11" s="18"/>
       <c r="E11" s="18"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
+      <c r="F11" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="H11" s="12">
+        <v>0</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
@@ -17209,97 +15634,77 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:I111" xr:uid="{776C4DE2-2957-440A-A09D-B0AB3152981D}">
-    <sortState ref="A2:I120">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I120">
       <sortCondition ref="A1:A111"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="C1:E60 A62:I109 A2:I60">
-    <cfRule type="expression" dxfId="67" priority="29">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A62:I109 A2:I60">
-    <cfRule type="expression" dxfId="66" priority="30">
+  <conditionalFormatting sqref="A61">
+    <cfRule type="expression" dxfId="44" priority="11">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A88:A106 C88:E106">
-    <cfRule type="expression" dxfId="65" priority="32">
+    <cfRule type="expression" dxfId="43" priority="32">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A61:D61 F61:H61">
+    <cfRule type="expression" dxfId="42" priority="3">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="41" priority="4">
+      <formula>COLUMN()=CELL("col")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:I1">
+    <cfRule type="expression" dxfId="40" priority="16">
+      <formula>COLUMN()=CELL("col")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:I60 A62:I109">
+    <cfRule type="expression" dxfId="39" priority="30">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:I60 C1:E60 A62:I109">
+    <cfRule type="expression" dxfId="38" priority="29">
+      <formula>COLUMN()=CELL("col")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A110:I300">
+    <cfRule type="expression" dxfId="37" priority="1">
+      <formula>COLUMN()=CELL("col")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="2">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C90">
-    <cfRule type="expression" dxfId="64" priority="114">
+    <cfRule type="expression" dxfId="35" priority="114">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C88:E105">
-    <cfRule type="expression" dxfId="63" priority="93">
+  <conditionalFormatting sqref="E3:E106">
+    <cfRule type="expression" dxfId="34" priority="5">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E60 E62:E106">
-    <cfRule type="expression" dxfId="62" priority="28">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:I1">
-    <cfRule type="expression" dxfId="61" priority="16">
+  <conditionalFormatting sqref="E61">
+    <cfRule type="expression" dxfId="33" priority="6">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G25">
-    <cfRule type="expression" dxfId="60" priority="17">
+    <cfRule type="expression" dxfId="32" priority="17">
       <formula>OR(ROW()=CELL("row"),col()=CELL("col"))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A61:B61">
-    <cfRule type="expression" dxfId="59" priority="9">
+  <conditionalFormatting sqref="H61:I61">
+    <cfRule type="expression" dxfId="31" priority="7">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="10">
+    <cfRule type="expression" dxfId="30" priority="8">
       <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A61">
-    <cfRule type="expression" dxfId="57" priority="11">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C61:D61 F61:H61">
-    <cfRule type="expression" dxfId="56" priority="4">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C61:D61 F61:H61">
-    <cfRule type="expression" dxfId="55" priority="3">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E61">
-    <cfRule type="expression" dxfId="54" priority="5">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="53" priority="6">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H61:I61">
-    <cfRule type="expression" dxfId="52" priority="7">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="51" priority="8">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A110:I300">
-    <cfRule type="expression" dxfId="50" priority="1">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A110:I300">
-    <cfRule type="expression" dxfId="49" priority="2">
-      <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -17313,8 +15718,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:I300"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G95" sqref="G95"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17519,11 +15924,15 @@
         <f>A11=Metadata!A11</f>
         <v>1</v>
       </c>
-      <c r="C11" s="23"/>
+      <c r="C11" s="23" t="s">
+        <v>336</v>
+      </c>
       <c r="D11" s="24"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
-      <c r="G11" s="12"/>
+      <c r="G11" s="12" t="s">
+        <v>249</v>
+      </c>
       <c r="H11" s="27"/>
       <c r="I11" s="20"/>
     </row>
@@ -21743,114 +20152,86 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:I109" xr:uid="{44BD8FFD-EDA1-47AD-AC03-3890015323F4}">
-    <sortState ref="A2:I120">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I120">
       <sortCondition ref="A1:A109"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="A2:B94">
-    <cfRule type="expression" dxfId="48" priority="48">
+  <conditionalFormatting sqref="A77:A86">
+    <cfRule type="expression" dxfId="29" priority="50">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="49">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A88:A300">
+    <cfRule type="expression" dxfId="28" priority="11">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:B300">
+    <cfRule type="expression" dxfId="27" priority="9">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="10">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A77:A86 A88:A94">
-    <cfRule type="expression" dxfId="46" priority="50">
+  <conditionalFormatting sqref="C82:C88">
+    <cfRule type="expression" dxfId="25" priority="21">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C82:C88">
-    <cfRule type="expression" dxfId="45" priority="21">
+  <conditionalFormatting sqref="C95:H300">
+    <cfRule type="expression" dxfId="24" priority="3">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:I2 I56:I81 F64:F68 F69:H74 G75:H81 C64:D94 G82:I93 G94:H94 A1:I1 C3:F63 G56:H68 G3:I53 F75:F94">
-    <cfRule type="expression" dxfId="44" priority="20">
+    <cfRule type="expression" dxfId="23" priority="4">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:I2 I56:I81 F64:F68 F69:H74 G75:H81 C64:D94 G82:I93 G94:H94 C3:F63 G56:H68 G3:I53 F75:F94">
-    <cfRule type="expression" dxfId="43" priority="19">
+  <conditionalFormatting sqref="C2:I2 C3:F63 G56:H68 I56:I81 F64:F68 C64:E94 F69:H74 G75:H81 F75:F94 G82:I93 G94:H94 A1:I1">
+    <cfRule type="expression" dxfId="22" priority="20">
+      <formula>COLUMN()=CELL("col")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:I2 C3:F63 G56:H68 I56:I81 F64:F68 C64:E94 F69:H74 G75:H81 F75:F94 G82:I93 G94:H94">
+    <cfRule type="expression" dxfId="21" priority="19">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25:F25">
-    <cfRule type="expression" dxfId="42" priority="22">
+    <cfRule type="expression" dxfId="20" priority="22">
       <formula>OR(ROW()=CELL("row"),col()=CELL("col"))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E64:E94">
-    <cfRule type="expression" dxfId="41" priority="30">
+  <conditionalFormatting sqref="G81">
+    <cfRule type="expression" dxfId="19" priority="106">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="31">
+    <cfRule type="expression" dxfId="18" priority="107">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G81">
-    <cfRule type="expression" dxfId="39" priority="106">
+  <conditionalFormatting sqref="G3:I55">
+    <cfRule type="expression" dxfId="17" priority="1">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="107">
+    <cfRule type="expression" dxfId="16" priority="2">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H94:I94">
-    <cfRule type="expression" dxfId="37" priority="36">
+    <cfRule type="expression" dxfId="15" priority="36">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="37">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A95:B300">
-    <cfRule type="expression" dxfId="35" priority="9">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="34" priority="10">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A95:A300">
-    <cfRule type="expression" dxfId="33" priority="11">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F95:H300 C95:D300">
-    <cfRule type="expression" dxfId="32" priority="4">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F95:H300 C95:D300">
-    <cfRule type="expression" dxfId="31" priority="3">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E95:E300">
-    <cfRule type="expression" dxfId="30" priority="5">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="29" priority="6">
+    <cfRule type="expression" dxfId="14" priority="37">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H95:I300">
-    <cfRule type="expression" dxfId="28" priority="7">
+    <cfRule type="expression" dxfId="13" priority="7">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="8">
+    <cfRule type="expression" dxfId="12" priority="8">
       <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G54:I55">
-    <cfRule type="expression" dxfId="26" priority="2">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G54:I55">
-    <cfRule type="expression" dxfId="25" priority="1">
-      <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -21864,8 +20245,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:I300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22118,7 +20499,9 @@
         <v>273</v>
       </c>
       <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
+      <c r="F11" s="12" t="s">
+        <v>282</v>
+      </c>
       <c r="G11" s="12"/>
       <c r="H11" s="12" t="s">
         <v>327</v>
@@ -26787,99 +25170,38 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:I120" xr:uid="{9CD57A02-0363-4F86-9C3F-3BEF2ED54F1B}">
-    <sortState ref="A2:I120">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I120">
       <sortCondition ref="A1:A120"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="A2:B107">
-    <cfRule type="expression" dxfId="24" priority="34">
+  <conditionalFormatting sqref="A77:A86">
+    <cfRule type="expression" dxfId="11" priority="36">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="35">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A88:A300">
+    <cfRule type="expression" dxfId="10" priority="12">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:I300">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A77:A86 A88:A107">
-    <cfRule type="expression" dxfId="22" priority="36">
+  <conditionalFormatting sqref="A2:I300">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:I1 C2:I107">
-    <cfRule type="expression" dxfId="21" priority="21">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:I107">
-    <cfRule type="expression" dxfId="20" priority="20">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E106:E107">
-    <cfRule type="expression" dxfId="19" priority="22">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A108:B300">
-    <cfRule type="expression" dxfId="18" priority="10">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="17" priority="11">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A108:A300">
-    <cfRule type="expression" dxfId="16" priority="12">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C109:I109 C108:G108 I108 C112:I112 C110:G111 I110:I111 C114:I300 C113:G113 I113">
-    <cfRule type="expression" dxfId="15" priority="8">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C109:I109 C108:G108 I108 C112:I112 C110:G111 I110:I111 C114:I300 C113:G113 I113">
-    <cfRule type="expression" dxfId="14" priority="7">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E108:E300">
-    <cfRule type="expression" dxfId="13" priority="9">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H108">
-    <cfRule type="expression" dxfId="12" priority="6">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H108">
-    <cfRule type="expression" dxfId="11" priority="5">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H110:H111">
-    <cfRule type="expression" dxfId="10" priority="4">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H110:H111">
-    <cfRule type="expression" dxfId="9" priority="3">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H113">
-    <cfRule type="expression" dxfId="8" priority="2">
-      <formula>COLUMN()=CELL("col")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H113">
-    <cfRule type="expression" dxfId="7" priority="1">
+  <conditionalFormatting sqref="E106:E300">
+    <cfRule type="expression" dxfId="7" priority="9">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -27957,7 +26279,7 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="37">
         <f ca="1">NOW()</f>
-        <v>45680.752327430557</v>
+        <v>45729.781559143521</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
included ATC and Crete
</commit_message>
<xml_diff>
--- a/exso/Files/ReportsInfo.xlsx
+++ b/exso/Files/ReportsInfo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.natsikas\Desktop\Admie-Desktop\Projects\exso\exso\exso\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thanos\Desktop\Admie-Desktop\Projects\exso\exso\exso\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D2E72F-8D6B-4644-BFC4-7A898FE28E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87A361F-F7FE-40D0-B0F1-EF6FAC4C7353}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,19 +26,8 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Read Settings'!$A$1:$I$111</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Time Settings'!$A$1:$I$120</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -50,6 +39,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
+    <author>Thanos</author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
@@ -76,6 +66,30 @@
           <t>NOT YET IMPLEMENTED:
 Alias feature is a (unique) nickname given to the official report name, which will be used as an intechangeable tag of the official report name. 
 Currently, the "Report Name" itself is the alias (although in most cases, it's identical to the official report-name)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F10" authorId="1" shapeId="0" xr:uid="{0C07F9CF-50DA-48C6-BF10-24C4FC2A23BC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Thanos:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+evenway before, but needs handling of different parsing behaviour&amp; renaming</t>
         </r>
       </text>
     </comment>
@@ -1184,7 +1198,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2000" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2005" uniqueCount="338">
   <si>
     <t>Report Name</t>
   </si>
@@ -2199,6 +2213,9 @@
   </si>
   <si>
     <t>DailyDispatchOfCreteElectricalSystem.txt</t>
+  </si>
+  <si>
+    <t>['ATC']</t>
   </si>
 </sst>
 </file>
@@ -2210,7 +2227,7 @@
     <numFmt numFmtId="165" formatCode="h:mm"/>
     <numFmt numFmtId="166" formatCode="m/d/yyyy\ h:mm"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2245,6 +2262,19 @@
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -3640,9 +3670,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3680,7 +3710,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3786,7 +3816,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3928,7 +3958,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3940,7 +3970,7 @@
   <dimension ref="A1:L300"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4285,7 +4315,7 @@
         <v>176</v>
       </c>
       <c r="F10" s="40">
-        <v>42005</v>
+        <v>44005</v>
       </c>
       <c r="G10" s="48"/>
       <c r="H10" s="8" t="b">
@@ -4297,8 +4327,7 @@
         <v>1</v>
       </c>
       <c r="J10" s="13" t="b">
-        <f>IF(Metadata!H10="",TRUE(),FALSE())</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10" s="14" t="s">
         <v>30</v>
@@ -10608,7 +10637,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:L120" xr:uid="{D0972C50-907B-4A2C-82F0-ED51F06329AA}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L120">
+    <sortState ref="A2:L120">
       <sortCondition ref="A2:A120"/>
     </sortState>
   </autoFilter>
@@ -10937,7 +10966,7 @@
   <dimension ref="A1:I300"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11144,12 +11173,20 @@
         <f>Metadata!A10=A10</f>
         <v>1</v>
       </c>
-      <c r="C10" s="8"/>
+      <c r="C10" s="8" t="s">
+        <v>185</v>
+      </c>
       <c r="D10" s="18"/>
       <c r="E10" s="18"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="12"/>
+      <c r="F10" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>337</v>
+      </c>
+      <c r="H10" s="12">
+        <v>0</v>
+      </c>
       <c r="I10" s="12"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -15634,7 +15671,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:I111" xr:uid="{776C4DE2-2957-440A-A09D-B0AB3152981D}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I120">
+    <sortState ref="A2:I120">
       <sortCondition ref="A1:A111"/>
     </sortState>
   </autoFilter>
@@ -15719,7 +15756,7 @@
   <dimension ref="A1:I300"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15912,9 +15949,15 @@
       <c r="D10" s="24"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="20"/>
+      <c r="G10" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="H10" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" s="20" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
@@ -20152,7 +20195,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:I109" xr:uid="{44BD8FFD-EDA1-47AD-AC03-3890015323F4}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I120">
+    <sortState ref="A2:I120">
       <sortCondition ref="A1:A109"/>
     </sortState>
   </autoFilter>
@@ -20246,7 +20289,7 @@
   <dimension ref="A1:I300"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20477,8 +20520,12 @@
         <v>273</v>
       </c>
       <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
+      <c r="F10" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="G10" s="12">
+        <v>0</v>
+      </c>
       <c r="H10" s="12" t="s">
         <v>327</v>
       </c>
@@ -25170,7 +25217,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:I120" xr:uid="{9CD57A02-0363-4F86-9C3F-3BEF2ED54F1B}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I120">
+    <sortState ref="A2:I120">
       <sortCondition ref="A1:A120"/>
     </sortState>
   </autoFilter>
@@ -26279,7 +26326,7 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="37">
         <f ca="1">NOW()</f>
-        <v>45729.781559143521</v>
+        <v>45734.941099884258</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>